<commit_message>
fix single quoted sheet names
</commit_message>
<xml_diff>
--- a/test/tias.xlsx
+++ b/test/tias.xlsx
@@ -5,10 +5,10 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
-    <sheet name="This is a sheet" sheetId="1" state="visible" r:id="rId2"/>
+    <sheet name="This is a - sheet" sheetId="1" state="visible" r:id="rId2"/>
     <sheet name="Sheet2" sheetId="2" state="visible" r:id="rId3"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
@@ -30,6 +30,7 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -96,12 +97,12 @@
     </xf>
   </cellXfs>
   <cellStyles count="6">
-    <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="false"/>
-    <cellStyle name="Comma" xfId="15" builtinId="3" customBuiltin="false"/>
-    <cellStyle name="Comma [0]" xfId="16" builtinId="6" customBuiltin="false"/>
-    <cellStyle name="Currency" xfId="17" builtinId="4" customBuiltin="false"/>
-    <cellStyle name="Currency [0]" xfId="18" builtinId="7" customBuiltin="false"/>
-    <cellStyle name="Percent" xfId="19" builtinId="5" customBuiltin="false"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Comma" xfId="15" builtinId="3"/>
+    <cellStyle name="Comma [0]" xfId="16" builtinId="6"/>
+    <cellStyle name="Currency" xfId="17" builtinId="4"/>
+    <cellStyle name="Currency [0]" xfId="18" builtinId="7"/>
+    <cellStyle name="Percent" xfId="19" builtinId="5"/>
   </cellStyles>
 </styleSheet>
 </file>
@@ -113,7 +114,7 @@
   </sheetPr>
   <dimension ref="B2:C2"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="C3" activeCellId="0" sqref="C3"/>
     </sheetView>
   </sheetViews>
@@ -148,7 +149,7 @@
   </sheetPr>
   <dimension ref="B3:C6"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="B3" activeCellId="0" sqref="B3"/>
     </sheetView>
   </sheetViews>
@@ -159,7 +160,7 @@
   <sheetData>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B3" s="0" t="n">
-        <f aca="false">'This is a sheet'!$B$2*C6*1.05</f>
+        <f aca="false">'This is a - sheet'!$B$2*C6*1.05</f>
         <v>15.75</v>
       </c>
     </row>
@@ -171,7 +172,7 @@
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>

</xml_diff>